<commit_message>
Se crean las Historias de Usuario
se realizo con:
-Brandon estiben Morales
-Jesus Andres Gonzalez
-Juan Diego Rios
</commit_message>
<xml_diff>
--- a/Documentos/Historias de Usuarios - CESPB.xlsx
+++ b/Documentos/Historias de Usuarios - CESPB.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Rol</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Registrar Usuario</t>
   </si>
   <si>
-    <t xml:space="preserve">Tener los usuarios en la base de datos </t>
-  </si>
-  <si>
     <t>Usuario Admin/Invitado</t>
   </si>
   <si>
@@ -76,6 +73,15 @@
   </si>
   <si>
     <t>MEDIA</t>
+  </si>
+  <si>
+    <t>Registrar Personal</t>
+  </si>
+  <si>
+    <t>Tener los usuarios en la base de datos para el ingreso del aplicativo</t>
+  </si>
+  <si>
+    <t>Tener el personal en la base de datos para el control de entrada y salida</t>
   </si>
 </sst>
 </file>
@@ -631,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +666,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -669,36 +675,36 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -708,16 +714,16 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>5</v>
@@ -725,17 +731,33 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>